<commit_message>
Add two-stage screening: title+abstract then full-text via PMC for all databases
Previously only PubMed had full-text screening via PMC. Now all four
databases (PubMed, Scopus, ACM, IEEE) use a shared two-stage pipeline:
1. Title+Abstract screening (stage 1)
2. Full-text screening via PMC DOI/PMID lookup (stage 2)

Papers without available PMC full text pass through automatically.
Moved PMC functions (batch_get_pmcids, fetch_pmc_fulltext) to
shared_screening.py and added run_fulltext_screening() for reuse.

Results: PubMed 708, Scopus 933, ACM 16, IEEE 23 → 1256 unique after dedup.

https://claude.ai/code/session_0183JkTrfns2hjtTL6Xwo5in
</commit_message>
<xml_diff>
--- a/ACM_Screening_Results.xlsx
+++ b/ACM_Screening_Results.xlsx
@@ -982,7 +982,7 @@
       </c>
       <c r="J2" s="7" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K2" s="7" t="inlineStr">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="J3" s="8" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K3" s="8" t="inlineStr">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="J4" s="7" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K4" s="7" t="inlineStr">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="J5" s="8" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K5" s="8" t="inlineStr">
@@ -1414,7 +1414,7 @@
       </c>
       <c r="J6" s="7" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K6" s="7" t="inlineStr">
@@ -1522,7 +1522,7 @@
       </c>
       <c r="J7" s="8" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K7" s="8" t="inlineStr">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="J8" s="7" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K8" s="7" t="inlineStr">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="J9" s="8" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K9" s="8" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="J10" s="7" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K10" s="7" t="inlineStr">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="J11" s="8" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K11" s="8" t="inlineStr">
@@ -2062,7 +2062,7 @@
       </c>
       <c r="J12" s="7" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K12" s="7" t="inlineStr">
@@ -2170,7 +2170,7 @@
       </c>
       <c r="J13" s="8" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K13" s="8" t="inlineStr">
@@ -2278,7 +2278,7 @@
       </c>
       <c r="J14" s="7" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K14" s="7" t="inlineStr">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="J15" s="8" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K15" s="8" t="inlineStr">
@@ -2494,7 +2494,7 @@
       </c>
       <c r="J16" s="7" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K16" s="7" t="inlineStr">
@@ -2602,7 +2602,7 @@
       </c>
       <c r="J17" s="8" t="inlineStr">
         <is>
-          <t>No full text available — passed through</t>
+          <t>No PMC full text — passed through</t>
         </is>
       </c>
       <c r="K17" s="8" t="inlineStr">

</xml_diff>